<commit_message>
re-designing the team profile page to look better. updating spreads
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week12.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week12.xlsx
@@ -841,59 +841,59 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6:45 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mississippi State</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>32.8</v>
+        <v>25</v>
       </c>
       <c r="H6" t="n">
-        <v>21.6</v>
+        <v>21.8</v>
       </c>
       <c r="I6" t="n">
-        <v>73.76000000000001</v>
+        <v>55.32</v>
       </c>
       <c r="J6" t="n">
-        <v>8.800000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="K6" t="n">
-        <v>4.199999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Missouri -6.5</t>
+          <t>Washington State -6.5</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Missouri -7.0</t>
+          <t>Washington State -7.5</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Missouri -11.2</t>
+          <t>Washington State -3.3</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>11.2</v>
+        <v>3.3</v>
       </c>
       <c r="P6" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -913,59 +913,59 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>6:45 PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>26</v>
+        <v>32.8</v>
       </c>
       <c r="H7" t="n">
-        <v>37.2</v>
+        <v>21.6</v>
       </c>
       <c r="I7" t="n">
-        <v>20.81</v>
+        <v>73.76000000000001</v>
       </c>
       <c r="J7" t="n">
-        <v>3.4</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K7" t="n">
         <v>4.199999999999999</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Marshall -6.5</t>
+          <t>Missouri -6.5</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Marshall -7.0</t>
+          <t>Missouri -7.0</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Marshall -11.2</t>
+          <t>Missouri -11.2</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>-11.2</v>
+        <v>11.2</v>
       </c>
       <c r="P7" t="n">
-        <v>-7</v>
+        <v>7</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -985,59 +985,59 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>1:00 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>15.8</v>
+        <v>26</v>
       </c>
       <c r="H8" t="n">
-        <v>38.6</v>
+        <v>37.2</v>
       </c>
       <c r="I8" t="n">
-        <v>6.88</v>
+        <v>20.81</v>
       </c>
       <c r="J8" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="K8" t="n">
         <v>4.199999999999999</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Kansas State -20.0</t>
+          <t>Marshall -6.5</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Kansas State -18.5</t>
+          <t>Marshall -7.0</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Kansas State -22.7</t>
+          <t>Marshall -11.2</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>-22.7</v>
+        <v>-11.2</v>
       </c>
       <c r="P8" t="n">
-        <v>-18.5</v>
+        <v>-7</v>
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -1062,54 +1062,54 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>39.8</v>
+        <v>15.8</v>
       </c>
       <c r="H9" t="n">
-        <v>6.6</v>
+        <v>38.6</v>
       </c>
       <c r="I9" t="n">
-        <v>96.88</v>
+        <v>6.88</v>
       </c>
       <c r="J9" t="n">
-        <v>5.4</v>
+        <v>3.1</v>
       </c>
       <c r="K9" t="n">
-        <v>4.100000000000001</v>
+        <v>4.199999999999999</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Indiana -30.5</t>
+          <t>Kansas State -20.0</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Indiana -29.0</t>
+          <t>Kansas State -18.5</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Indiana -33.1</t>
+          <t>Kansas State -22.7</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>33.1</v>
+        <v>-22.7</v>
       </c>
       <c r="P9" t="n">
-        <v>29</v>
+        <v>-18.5</v>
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1197,63 +1197,63 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45976</v>
+        <v>45972</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Akron</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Kent State</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>15.6</v>
+        <v>28.2</v>
       </c>
       <c r="H11" t="n">
-        <v>29.6</v>
+        <v>19.2</v>
       </c>
       <c r="I11" t="n">
-        <v>18.33</v>
+        <v>68.94</v>
       </c>
       <c r="J11" t="n">
-        <v>7.8</v>
+        <v>3.9</v>
       </c>
       <c r="K11" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Michigan -10.0</t>
+          <t>Akron -5.0</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Michigan -10.0</t>
+          <t>Akron -5.0</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Michigan -14.0</t>
+          <t>Akron -9.1</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>-14</v>
+        <v>9.1</v>
       </c>
       <c r="P11" t="n">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -1273,59 +1273,59 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>37.1</v>
+        <v>15.6</v>
       </c>
       <c r="H12" t="n">
-        <v>29.7</v>
+        <v>29.6</v>
       </c>
       <c r="I12" t="n">
-        <v>64.70999999999999</v>
+        <v>18.33</v>
       </c>
       <c r="J12" t="n">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
       <c r="K12" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>UNLV -4.5</t>
+          <t>Michigan -10.0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>UNLV -3.5</t>
+          <t>Michigan -10.0</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>UNLV -7.4</t>
+          <t>Michigan -14.0</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>7.4</v>
+        <v>-14</v>
       </c>
       <c r="P12" t="n">
-        <v>3.5</v>
+        <v>-10</v>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>9:00 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1427,49 +1427,49 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>25</v>
+        <v>24.4</v>
       </c>
       <c r="H14" t="n">
-        <v>21.8</v>
+        <v>27</v>
       </c>
       <c r="I14" t="n">
-        <v>55.32</v>
+        <v>40.3</v>
       </c>
       <c r="J14" t="n">
-        <v>8.1</v>
+        <v>5.3</v>
       </c>
       <c r="K14" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Washington State -6.5</t>
+          <t>Oregon State -1.0</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Washington State -7.0</t>
+          <t>Tulsa -1.0</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Washington State -3.3</t>
+          <t>Oregon State -2.5</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>3.3</v>
+        <v>-2.5</v>
       </c>
       <c r="P14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1485,63 +1485,63 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45972</v>
+        <v>45975</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Akron</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Kent State</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>28.2</v>
+        <v>36.8</v>
       </c>
       <c r="H15" t="n">
-        <v>19.2</v>
+        <v>9.5</v>
       </c>
       <c r="I15" t="n">
-        <v>68.94</v>
+        <v>94.25</v>
       </c>
       <c r="J15" t="n">
-        <v>3.9</v>
+        <v>6.7</v>
       </c>
       <c r="K15" t="n">
-        <v>3.6</v>
+        <v>3.300000000000001</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Akron -5.0</t>
+          <t>Oregon -23.0</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Akron -5.5</t>
+          <t>Oregon -24.0</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Akron -9.1</t>
+          <t>Oregon -27.3</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>9.1</v>
+        <v>27.3</v>
       </c>
       <c r="P15" t="n">
-        <v>5.5</v>
+        <v>24</v>
       </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1561,59 +1561,59 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>3:15 PM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>32.4</v>
+        <v>46.7</v>
       </c>
       <c r="H16" t="n">
-        <v>17.8</v>
+        <v>10.5</v>
       </c>
       <c r="I16" t="n">
-        <v>80.09999999999999</v>
+        <v>97.8</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>2.9</v>
       </c>
       <c r="K16" t="n">
-        <v>3.5</v>
+        <v>3.299999999999997</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Arizona State -11.0</t>
+          <t>Tennessee -38.5</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Arizona State -11.0</t>
+          <t>Tennessee -39.5</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Arizona State -14.5</t>
+          <t>Tennessee -36.2</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>14.5</v>
+        <v>36.2</v>
       </c>
       <c r="P16" t="n">
-        <v>11</v>
+        <v>39.5</v>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -1633,59 +1633,59 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>24.4</v>
+        <v>43.2</v>
       </c>
       <c r="H17" t="n">
-        <v>27</v>
+        <v>8.4</v>
       </c>
       <c r="I17" t="n">
-        <v>40.3</v>
+        <v>97.38</v>
       </c>
       <c r="J17" t="n">
         <v>5.3</v>
       </c>
       <c r="K17" t="n">
-        <v>3.5</v>
+        <v>3.200000000000003</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Oregon State -1.0</t>
+          <t>Ohio State -31.5</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Tulsa -1.0</t>
+          <t>Ohio State -31.5</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Oregon State -2.5</t>
+          <t>Ohio State -34.7</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>-2.5</v>
+        <v>34.7</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>31.5</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1701,63 +1701,63 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>36.8</v>
+        <v>39.8</v>
       </c>
       <c r="H18" t="n">
-        <v>9.5</v>
+        <v>6.6</v>
       </c>
       <c r="I18" t="n">
-        <v>94.25</v>
+        <v>96.88</v>
       </c>
       <c r="J18" t="n">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="K18" t="n">
-        <v>3.300000000000001</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Oregon -23.0</t>
+          <t>Indiana -30.5</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Oregon -24.0</t>
+          <t>Indiana -30.0</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Oregon -27.3</t>
+          <t>Indiana -33.1</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>27.3</v>
+        <v>33.1</v>
       </c>
       <c r="P18" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1777,59 +1777,59 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:15 PM</t>
+          <t>3:30 PM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>46.7</v>
+        <v>25.6</v>
       </c>
       <c r="H19" t="n">
-        <v>10.5</v>
+        <v>16</v>
       </c>
       <c r="I19" t="n">
-        <v>97.8</v>
+        <v>71.06999999999999</v>
       </c>
       <c r="J19" t="n">
-        <v>2.9</v>
+        <v>7.2</v>
       </c>
       <c r="K19" t="n">
-        <v>3.299999999999997</v>
+        <v>3.1</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Tennessee -38.5</t>
+          <t>Wake Forest -6.0</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Tennessee -39.5</t>
+          <t>Wake Forest -6.5</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Tennessee -36.2</t>
+          <t>Wake Forest -9.6</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>36.2</v>
+        <v>9.6</v>
       </c>
       <c r="P19" t="n">
-        <v>39.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -1849,59 +1849,59 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>43.2</v>
+        <v>32.4</v>
       </c>
       <c r="H20" t="n">
-        <v>8.4</v>
+        <v>17.8</v>
       </c>
       <c r="I20" t="n">
-        <v>97.38</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>5.3</v>
+        <v>7</v>
       </c>
       <c r="K20" t="n">
-        <v>3.200000000000003</v>
+        <v>3</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Ohio State -31.5</t>
+          <t>Arizona State -11.0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Ohio State -31.5</t>
+          <t>Arizona State -11.5</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Ohio State -34.7</t>
+          <t>Arizona State -14.5</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>34.7</v>
+        <v>14.5</v>
       </c>
       <c r="P20" t="n">
-        <v>31.5</v>
+        <v>11.5</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -1921,59 +1921,59 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>25.6</v>
+        <v>37.1</v>
       </c>
       <c r="H21" t="n">
-        <v>16</v>
+        <v>29.7</v>
       </c>
       <c r="I21" t="n">
-        <v>71.06999999999999</v>
+        <v>64.70999999999999</v>
       </c>
       <c r="J21" t="n">
-        <v>7.2</v>
+        <v>7.6</v>
       </c>
       <c r="K21" t="n">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Wake Forest -6.0</t>
+          <t>UNLV -4.5</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Wake Forest -6.5</t>
+          <t>UNLV -4.5</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Wake Forest -9.6</t>
+          <t>UNLV -7.4</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>9.6</v>
+        <v>7.4</v>
       </c>
       <c r="P21" t="n">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -2209,59 +2209,59 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>22.3</v>
+        <v>25.2</v>
       </c>
       <c r="H25" t="n">
-        <v>33.7</v>
+        <v>25.6</v>
       </c>
       <c r="I25" t="n">
-        <v>23.11</v>
+        <v>43.3</v>
       </c>
       <c r="J25" t="n">
-        <v>3.2</v>
+        <v>6.7</v>
       </c>
       <c r="K25" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Delaware -8.5</t>
+          <t>Kennesaw State -2.5</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Delaware -9.0</t>
+          <t>Kennesaw State -3.0</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Delaware -11.4</t>
+          <t>Kennesaw State -0.5</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>-11.4</v>
+        <v>-0.5</v>
       </c>
       <c r="P25" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -2281,59 +2281,59 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>23</v>
+        <v>36.2</v>
       </c>
       <c r="H26" t="n">
-        <v>43.4</v>
+        <v>26.8</v>
       </c>
       <c r="I26" t="n">
-        <v>8.640000000000001</v>
+        <v>69.66</v>
       </c>
       <c r="J26" t="n">
-        <v>3.6</v>
+        <v>7</v>
       </c>
       <c r="K26" t="n">
-        <v>2.399999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>North Texas -18.0</t>
+          <t>UConn -8.0</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>North Texas -18.0</t>
+          <t>UConn -7.0</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>North Texas -20.4</t>
+          <t>UConn -9.4</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>-20.4</v>
+        <v>9.4</v>
       </c>
       <c r="P26" t="n">
-        <v>-18</v>
+        <v>7</v>
       </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -2353,59 +2353,59 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>1:00 PM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>29.8</v>
+        <v>23</v>
       </c>
       <c r="H27" t="n">
-        <v>26.2</v>
+        <v>43.4</v>
       </c>
       <c r="I27" t="n">
-        <v>56.15</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="J27" t="n">
-        <v>9.300000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="K27" t="n">
-        <v>2.3</v>
+        <v>2.399999999999999</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Cincinnati -6.0</t>
+          <t>North Texas -18.0</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Cincinnati -6.0</t>
+          <t>North Texas -18.0</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Cincinnati -3.7</t>
+          <t>North Texas -20.4</t>
         </is>
       </c>
       <c r="O27" t="n">
-        <v>3.7</v>
+        <v>-20.4</v>
       </c>
       <c r="P27" t="n">
-        <v>6</v>
+        <v>-18</v>
       </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -2425,59 +2425,59 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>9:15 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>30.2</v>
+        <v>29.8</v>
       </c>
       <c r="H28" t="n">
-        <v>22.5</v>
+        <v>26.2</v>
       </c>
       <c r="I28" t="n">
-        <v>66.98999999999999</v>
+        <v>56.15</v>
       </c>
       <c r="J28" t="n">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K28" t="n">
         <v>2.3</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>BYU -6.0</t>
+          <t>Cincinnati -6.0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>BYU -5.5</t>
+          <t>Cincinnati -6.0</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>BYU -7.8</t>
+          <t>Cincinnati -3.7</t>
         </is>
       </c>
       <c r="O28" t="n">
-        <v>7.8</v>
+        <v>3.7</v>
       </c>
       <c r="P28" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -2497,59 +2497,59 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>9:15 PM</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>30</v>
+        <v>30.2</v>
       </c>
       <c r="H29" t="n">
-        <v>29.2</v>
+        <v>22.5</v>
       </c>
       <c r="I29" t="n">
-        <v>48.88</v>
+        <v>66.98999999999999</v>
       </c>
       <c r="J29" t="n">
-        <v>9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K29" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>East Carolina -3.0</t>
+          <t>BYU -6.0</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>East Carolina -3.0</t>
+          <t>BYU -5.5</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>East Carolina -0.9</t>
+          <t>BYU -7.8</t>
         </is>
       </c>
       <c r="O29" t="n">
-        <v>0.9</v>
+        <v>7.8</v>
       </c>
       <c r="P29" t="n">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2579,49 +2579,49 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>25.2</v>
+        <v>30</v>
       </c>
       <c r="H30" t="n">
-        <v>25.6</v>
+        <v>29.2</v>
       </c>
       <c r="I30" t="n">
-        <v>43.3</v>
+        <v>48.88</v>
       </c>
       <c r="J30" t="n">
-        <v>6.7</v>
+        <v>9</v>
       </c>
       <c r="K30" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Kennesaw State -2.5</t>
+          <t>East Carolina -3.0</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Kennesaw State -2.5</t>
+          <t>East Carolina -3.0</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Kennesaw State -0.5</t>
+          <t>East Carolina -0.9</t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
       <c r="P30" t="n">
-        <v>-2.5</v>
+        <v>3</v>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2651,49 +2651,49 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>24.2</v>
+        <v>22.3</v>
       </c>
       <c r="H31" t="n">
-        <v>30</v>
+        <v>33.7</v>
       </c>
       <c r="I31" t="n">
-        <v>32.27</v>
+        <v>23.11</v>
       </c>
       <c r="J31" t="n">
-        <v>4.1</v>
+        <v>3.2</v>
       </c>
       <c r="K31" t="n">
         <v>1.9</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>South Alabama -4.0</t>
+          <t>Delaware -8.5</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>South Alabama -4.0</t>
+          <t>Delaware -9.5</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>South Alabama -5.9</t>
+          <t>Delaware -11.4</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>-5.9</v>
+        <v>-11.4</v>
       </c>
       <c r="P31" t="n">
-        <v>-4</v>
+        <v>-9.5</v>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2713,59 +2713,59 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>35.6</v>
+        <v>24.2</v>
       </c>
       <c r="H32" t="n">
-        <v>16.8</v>
+        <v>30</v>
       </c>
       <c r="I32" t="n">
-        <v>86.45</v>
+        <v>32.27</v>
       </c>
       <c r="J32" t="n">
-        <v>6.8</v>
+        <v>4.1</v>
       </c>
       <c r="K32" t="n">
-        <v>1.800000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Washington -16.5</t>
+          <t>South Alabama -4.0</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Washington -17.0</t>
+          <t>South Alabama -4.0</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Washington -18.8</t>
+          <t>South Alabama -5.9</t>
         </is>
       </c>
       <c r="O32" t="n">
-        <v>18.8</v>
+        <v>-5.9</v>
       </c>
       <c r="P32" t="n">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -2781,7 +2781,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2790,54 +2790,54 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>22.2</v>
+        <v>35.6</v>
       </c>
       <c r="H33" t="n">
-        <v>21.5</v>
+        <v>16.8</v>
       </c>
       <c r="I33" t="n">
-        <v>49.16</v>
+        <v>86.45</v>
       </c>
       <c r="J33" t="n">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="K33" t="n">
-        <v>1.7</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Central Michigan -2.0</t>
+          <t>Washington -16.5</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Central Michigan -2.5</t>
+          <t>Washington -17.0</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Central Michigan -0.8</t>
+          <t>Washington -18.8</t>
         </is>
       </c>
       <c r="O33" t="n">
-        <v>0.8</v>
+        <v>18.8</v>
       </c>
       <c r="P33" t="n">
-        <v>2.5</v>
+        <v>17</v>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -2853,63 +2853,63 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45976</v>
+        <v>45973</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>20.8</v>
+        <v>22.2</v>
       </c>
       <c r="H34" t="n">
-        <v>39.9</v>
+        <v>21.5</v>
       </c>
       <c r="I34" t="n">
-        <v>9.859999999999999</v>
+        <v>49.16</v>
       </c>
       <c r="J34" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Central Michigan -2.0</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Central Michigan -2.5</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Central Michigan -0.8</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P34" t="n">
         <v>2.5</v>
-      </c>
-      <c r="K34" t="n">
-        <v>1.600000000000001</v>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>UTSA -18.0</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>UTSA -17.5</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>UTSA -19.1</t>
-        </is>
-      </c>
-      <c r="O34" t="n">
-        <v>-19.1</v>
-      </c>
-      <c r="P34" t="n">
-        <v>-17.5</v>
       </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2939,49 +2939,49 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>27.8</v>
+        <v>20.8</v>
       </c>
       <c r="H35" t="n">
-        <v>22.2</v>
+        <v>39.9</v>
       </c>
       <c r="I35" t="n">
-        <v>60.51</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="J35" t="n">
-        <v>5.8</v>
+        <v>2.5</v>
       </c>
       <c r="K35" t="n">
-        <v>1.6</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Missouri State -4.0</t>
+          <t>UTSA -18.0</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Missouri State -4.0</t>
+          <t>UTSA -17.5</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Missouri State -5.6</t>
+          <t>UTSA -19.1</t>
         </is>
       </c>
       <c r="O35" t="n">
-        <v>5.6</v>
+        <v>-19.1</v>
       </c>
       <c r="P35" t="n">
-        <v>4</v>
+        <v>-17.5</v>
       </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -3001,59 +3001,59 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>11:45 AM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>32.7</v>
+        <v>27.8</v>
       </c>
       <c r="H36" t="n">
-        <v>25.4</v>
+        <v>22.2</v>
       </c>
       <c r="I36" t="n">
-        <v>64.97</v>
+        <v>60.51</v>
       </c>
       <c r="J36" t="n">
-        <v>9.199999999999999</v>
+        <v>5.8</v>
       </c>
       <c r="K36" t="n">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>LSU -6.5</t>
+          <t>Missouri State -4.0</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>LSU -6.0</t>
+          <t>Missouri State -4.0</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>LSU -7.3</t>
+          <t>Missouri State -5.6</t>
         </is>
       </c>
       <c r="O36" t="n">
-        <v>7.3</v>
+        <v>5.6</v>
       </c>
       <c r="P36" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -3073,59 +3073,59 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>9:30 PM</t>
+          <t>11:45 AM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>25.8</v>
+        <v>32.7</v>
       </c>
       <c r="H37" t="n">
-        <v>20.6</v>
+        <v>25.4</v>
       </c>
       <c r="I37" t="n">
-        <v>59.7</v>
+        <v>64.97</v>
       </c>
       <c r="J37" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>LSU -6.5</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>LSU -6.0</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>LSU -7.3</t>
+        </is>
+      </c>
+      <c r="O37" t="n">
         <v>7.3</v>
       </c>
-      <c r="K37" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>Fresno State -4.0</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>Fresno State -4.0</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>Fresno State -5.2</t>
-        </is>
-      </c>
-      <c r="O37" t="n">
-        <v>5.2</v>
-      </c>
       <c r="P37" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3227,49 +3227,49 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Ball State</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Eastern Michigan</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>39</v>
+        <v>25.5</v>
       </c>
       <c r="H39" t="n">
-        <v>21.8</v>
+        <v>26.9</v>
       </c>
       <c r="I39" t="n">
-        <v>84.34999999999999</v>
+        <v>43.3</v>
       </c>
       <c r="J39" t="n">
-        <v>5.2</v>
+        <v>4.5</v>
       </c>
       <c r="K39" t="n">
-        <v>1.199999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Tulane -16.5</t>
+          <t>Eastern Michigan -3.0</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Tulane -16.0</t>
+          <t>Eastern Michigan -2.5</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Tulane -17.2</t>
+          <t>Eastern Michigan -1.4</t>
         </is>
       </c>
       <c r="O39" t="n">
-        <v>17.2</v>
+        <v>-1.4</v>
       </c>
       <c r="P39" t="n">
-        <v>16</v>
+        <v>-2.5</v>
       </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
@@ -3285,63 +3285,63 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45974</v>
+        <v>45976</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>32.6</v>
+        <v>21.4</v>
       </c>
       <c r="H40" t="n">
-        <v>22.4</v>
+        <v>30.4</v>
       </c>
       <c r="I40" t="n">
-        <v>72.66</v>
+        <v>24.96</v>
       </c>
       <c r="J40" t="n">
-        <v>6.9</v>
+        <v>3.9</v>
       </c>
       <c r="K40" t="n">
-        <v>1.199999999999999</v>
+        <v>1</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Old Dominion -10.0</t>
+          <t>San José State -8.5</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Old Dominion -11.5</t>
+          <t>San José State -8.0</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Old Dominion -10.3</t>
+          <t>San José State -9.0</t>
         </is>
       </c>
       <c r="O40" t="n">
-        <v>10.3</v>
+        <v>-9</v>
       </c>
       <c r="P40" t="n">
-        <v>11.5</v>
+        <v>-8</v>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -3357,63 +3357,63 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45976</v>
+        <v>45973</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Ball State</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Eastern Michigan</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>25.5</v>
+        <v>16</v>
       </c>
       <c r="H41" t="n">
-        <v>26.9</v>
+        <v>27.4</v>
       </c>
       <c r="I41" t="n">
-        <v>43.3</v>
+        <v>20.26</v>
       </c>
       <c r="J41" t="n">
-        <v>4.5</v>
+        <v>2.2</v>
       </c>
       <c r="K41" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Eastern Michigan -3.0</t>
+          <t>Northern Illinois -11.0</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Eastern Michigan -2.5</t>
+          <t>Northern Illinois -10.5</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Eastern Michigan -1.4</t>
+          <t>Northern Illinois -11.5</t>
         </is>
       </c>
       <c r="O41" t="n">
-        <v>-1.4</v>
+        <v>-11.5</v>
       </c>
       <c r="P41" t="n">
-        <v>-2.5</v>
+        <v>-10.5</v>
       </c>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
@@ -3429,63 +3429,63 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45976</v>
+        <v>45972</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>21.4</v>
+        <v>24.3</v>
       </c>
       <c r="H42" t="n">
-        <v>30.4</v>
+        <v>24.9</v>
       </c>
       <c r="I42" t="n">
-        <v>24.96</v>
+        <v>45.8</v>
       </c>
       <c r="J42" t="n">
-        <v>3.9</v>
+        <v>7.1</v>
       </c>
       <c r="K42" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>San José State -8.5</t>
+          <t>Ohio -1.5</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>San José State -8.0</t>
+          <t>Ohio -1.5</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>San José State -9.0</t>
+          <t>Ohio -0.6</t>
         </is>
       </c>
       <c r="O42" t="n">
-        <v>-9</v>
+        <v>-0.6</v>
       </c>
       <c r="P42" t="n">
-        <v>-8</v>
+        <v>-1.5</v>
       </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -3505,59 +3505,59 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>36.2</v>
+        <v>32.1</v>
       </c>
       <c r="H43" t="n">
-        <v>26.8</v>
+        <v>28.6</v>
       </c>
       <c r="I43" t="n">
-        <v>69.66</v>
+        <v>55.32</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="K43" t="n">
-        <v>0.9000000000000004</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>UConn -8.0</t>
+          <t>Georgia Southern -3.0</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>UConn -8.5</t>
+          <t>Georgia Southern -2.5</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>UConn -9.4</t>
+          <t>Georgia Southern -3.4</t>
         </is>
       </c>
       <c r="O43" t="n">
-        <v>9.4</v>
+        <v>3.4</v>
       </c>
       <c r="P43" t="n">
-        <v>8.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
@@ -3577,59 +3577,59 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>32.1</v>
+        <v>26.4</v>
       </c>
       <c r="H44" t="n">
-        <v>28.6</v>
+        <v>36.2</v>
       </c>
       <c r="I44" t="n">
-        <v>55.32</v>
+        <v>23.32</v>
       </c>
       <c r="J44" t="n">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="K44" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.0</t>
+          <t>South Florida -10.0</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Georgia Southern -2.5</t>
+          <t>South Florida -10.5</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.4</t>
+          <t>South Florida -9.7</t>
         </is>
       </c>
       <c r="O44" t="n">
-        <v>3.4</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="P44" t="n">
-        <v>2.5</v>
+        <v>-10.5</v>
       </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -3649,59 +3649,59 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>9:30 PM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>29.6</v>
+        <v>25.8</v>
       </c>
       <c r="H45" t="n">
-        <v>23.4</v>
+        <v>20.6</v>
       </c>
       <c r="I45" t="n">
-        <v>62.9</v>
+        <v>59.7</v>
       </c>
       <c r="J45" t="n">
-        <v>9.6</v>
+        <v>7.3</v>
       </c>
       <c r="K45" t="n">
-        <v>0.7999999999999998</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>USC -6.5</t>
+          <t>Fresno State -4.0</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>USC -7.0</t>
+          <t>Fresno State -4.5</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>USC -6.2</t>
+          <t>Fresno State -5.2</t>
         </is>
       </c>
       <c r="O45" t="n">
-        <v>6.2</v>
+        <v>5.2</v>
       </c>
       <c r="P45" t="n">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3803,49 +3803,49 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>27.8</v>
+        <v>22.4</v>
       </c>
       <c r="H47" t="n">
-        <v>21.4</v>
+        <v>33.3</v>
       </c>
       <c r="I47" t="n">
-        <v>62.64</v>
+        <v>21.56</v>
       </c>
       <c r="J47" t="n">
-        <v>9.699999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="K47" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5999999999999996</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Georgia -6.5</t>
+          <t>Notre Dame -10.5</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Georgia -6.0</t>
+          <t>Notre Dame -11.5</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Georgia -6.4</t>
+          <t>Notre Dame -10.9</t>
         </is>
       </c>
       <c r="O47" t="n">
-        <v>6.4</v>
+        <v>-10.9</v>
       </c>
       <c r="P47" t="n">
-        <v>6</v>
+        <v>-11.5</v>
       </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3875,49 +3875,49 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>22.4</v>
+        <v>27.8</v>
       </c>
       <c r="H48" t="n">
-        <v>33.3</v>
+        <v>21.4</v>
       </c>
       <c r="I48" t="n">
-        <v>21.56</v>
+        <v>62.64</v>
       </c>
       <c r="J48" t="n">
-        <v>8.9</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K48" t="n">
         <v>0.4000000000000004</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Notre Dame -10.5</t>
+          <t>Georgia -6.5</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Notre Dame -10.5</t>
+          <t>Georgia -6.0</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Notre Dame -10.9</t>
+          <t>Georgia -6.4</t>
         </is>
       </c>
       <c r="O48" t="n">
-        <v>-10.9</v>
+        <v>6.4</v>
       </c>
       <c r="P48" t="n">
-        <v>-10.5</v>
+        <v>6</v>
       </c>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
@@ -3933,63 +3933,63 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45972</v>
+        <v>45975</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>24.3</v>
+        <v>28</v>
       </c>
       <c r="H49" t="n">
-        <v>24.9</v>
+        <v>24</v>
       </c>
       <c r="I49" t="n">
-        <v>45.8</v>
+        <v>56.7</v>
       </c>
       <c r="J49" t="n">
-        <v>7.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K49" t="n">
-        <v>0.4</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Ohio -1.5</t>
+          <t>Louisville -3.5</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Ohio -1.0</t>
+          <t>Louisville -3.5</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Ohio -0.6</t>
+          <t>Louisville -3.9</t>
         </is>
       </c>
       <c r="O49" t="n">
-        <v>-0.6</v>
+        <v>3.9</v>
       </c>
       <c r="P49" t="n">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
@@ -4005,11 +4005,11 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4019,49 +4019,49 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>28</v>
+        <v>35.1</v>
       </c>
       <c r="H50" t="n">
-        <v>24</v>
+        <v>15.8</v>
       </c>
       <c r="I50" t="n">
-        <v>56.7</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="J50" t="n">
-        <v>9.300000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="K50" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Louisville -3.5</t>
+          <t>Texas A&amp;M -18.5</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Louisville -3.5</t>
+          <t>Texas A&amp;M -19.0</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Louisville -3.9</t>
+          <t>Texas A&amp;M -19.3</t>
         </is>
       </c>
       <c r="O50" t="n">
-        <v>3.9</v>
+        <v>19.3</v>
       </c>
       <c r="P50" t="n">
-        <v>3.5</v>
+        <v>19</v>
       </c>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
@@ -4081,59 +4081,59 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>35.1</v>
+        <v>21</v>
       </c>
       <c r="H51" t="n">
-        <v>15.8</v>
+        <v>37.8</v>
       </c>
       <c r="I51" t="n">
-        <v>87.34999999999999</v>
+        <v>12.29</v>
       </c>
       <c r="J51" t="n">
-        <v>8.1</v>
+        <v>5</v>
       </c>
       <c r="K51" t="n">
         <v>0.3000000000000007</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -18.5</t>
+          <t>Georgia Tech -16.5</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -19.0</t>
+          <t>Georgia Tech -17.0</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -19.3</t>
+          <t>Georgia Tech -16.7</t>
         </is>
       </c>
       <c r="O51" t="n">
-        <v>19.3</v>
+        <v>-16.7</v>
       </c>
       <c r="P51" t="n">
-        <v>19</v>
+        <v>-17</v>
       </c>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
@@ -4153,59 +4153,59 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>26.4</v>
+        <v>29.6</v>
       </c>
       <c r="H52" t="n">
-        <v>36.2</v>
+        <v>23.4</v>
       </c>
       <c r="I52" t="n">
-        <v>23.32</v>
+        <v>62.9</v>
       </c>
       <c r="J52" t="n">
-        <v>7.3</v>
+        <v>9.6</v>
       </c>
       <c r="K52" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>South Florida -10.0</t>
+          <t>USC -6.5</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>South Florida -10.0</t>
+          <t>USC -6.5</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>South Florida -9.7</t>
+          <t>USC -6.2</t>
         </is>
       </c>
       <c r="O52" t="n">
-        <v>-9.699999999999999</v>
+        <v>6.2</v>
       </c>
       <c r="P52" t="n">
-        <v>-10</v>
+        <v>6.5</v>
       </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
@@ -4230,54 +4230,54 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>21</v>
+        <v>34.6</v>
       </c>
       <c r="H53" t="n">
-        <v>37.8</v>
+        <v>28.9</v>
       </c>
       <c r="I53" t="n">
-        <v>12.29</v>
+        <v>62.37</v>
       </c>
       <c r="J53" t="n">
-        <v>5</v>
+        <v>7.3</v>
       </c>
       <c r="K53" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.2999999999999998</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Georgia Tech -16.5</t>
+          <t>Southern Miss -6.5</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.0</t>
+          <t>Southern Miss -6.0</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Georgia Tech -16.7</t>
+          <t>Southern Miss -5.7</t>
         </is>
       </c>
       <c r="O53" t="n">
-        <v>-16.7</v>
+        <v>5.7</v>
       </c>
       <c r="P53" t="n">
-        <v>-17</v>
+        <v>6</v>
       </c>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>4:00 PM</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4307,49 +4307,49 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>34.6</v>
+        <v>25.2</v>
       </c>
       <c r="H54" t="n">
-        <v>28.9</v>
+        <v>27.8</v>
       </c>
       <c r="I54" t="n">
-        <v>62.37</v>
+        <v>39.76</v>
       </c>
       <c r="J54" t="n">
-        <v>7.3</v>
+        <v>5.6</v>
       </c>
       <c r="K54" t="n">
         <v>0.2999999999999998</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Southern Miss -6.5</t>
+          <t>Liberty -3.0</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Southern Miss -6.0</t>
+          <t>Liberty -3.0</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Southern Miss -5.7</t>
+          <t>Liberty -2.7</t>
         </is>
       </c>
       <c r="O54" t="n">
-        <v>5.7</v>
+        <v>-2.7</v>
       </c>
       <c r="P54" t="n">
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr"/>
@@ -4369,59 +4369,59 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>4:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>25.2</v>
+        <v>27.2</v>
       </c>
       <c r="H55" t="n">
-        <v>27.8</v>
+        <v>20.5</v>
       </c>
       <c r="I55" t="n">
-        <v>39.76</v>
+        <v>62.9</v>
       </c>
       <c r="J55" t="n">
-        <v>5.6</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K55" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.2000000000000002</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Liberty -3.0</t>
+          <t>Alabama -7.0</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Liberty -3.0</t>
+          <t>Alabama -6.5</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Liberty -2.7</t>
+          <t>Alabama -6.7</t>
         </is>
       </c>
       <c r="O55" t="n">
-        <v>-2.7</v>
+        <v>6.7</v>
       </c>
       <c r="P55" t="n">
-        <v>-3</v>
+        <v>6.5</v>
       </c>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
@@ -4441,59 +4441,59 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>27.2</v>
+        <v>39</v>
       </c>
       <c r="H56" t="n">
-        <v>20.5</v>
+        <v>21.8</v>
       </c>
       <c r="I56" t="n">
-        <v>62.9</v>
+        <v>84.34999999999999</v>
       </c>
       <c r="J56" t="n">
-        <v>9.699999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="K56" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Alabama -7.0</t>
+          <t>Tulane -16.5</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Alabama -6.5</t>
+          <t>Tulane -17.0</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Alabama -6.7</t>
+          <t>Tulane -17.2</t>
         </is>
       </c>
       <c r="O56" t="n">
-        <v>6.7</v>
+        <v>17.2</v>
       </c>
       <c r="P56" t="n">
-        <v>6.5</v>
+        <v>17</v>
       </c>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr"/>
@@ -4509,63 +4509,63 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45976</v>
+        <v>45974</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>36.3</v>
+        <v>32.6</v>
       </c>
       <c r="H57" t="n">
-        <v>12.7</v>
+        <v>22.4</v>
       </c>
       <c r="I57" t="n">
-        <v>91.62</v>
+        <v>72.66</v>
       </c>
       <c r="J57" t="n">
-        <v>7.3</v>
+        <v>6.9</v>
       </c>
       <c r="K57" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Texas Tech -23.5</t>
+          <t>Old Dominion -10.0</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Texas Tech -23.5</t>
+          <t>Old Dominion -10.5</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Texas Tech -23.6</t>
+          <t>Old Dominion -10.3</t>
         </is>
       </c>
       <c r="O57" t="n">
-        <v>23.6</v>
+        <v>10.3</v>
       </c>
       <c r="P57" t="n">
-        <v>23.5</v>
+        <v>10.5</v>
       </c>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr"/>
@@ -4581,63 +4581,63 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>16</v>
+        <v>36.3</v>
       </c>
       <c r="H58" t="n">
-        <v>27.4</v>
+        <v>12.7</v>
       </c>
       <c r="I58" t="n">
-        <v>20.26</v>
+        <v>91.62</v>
       </c>
       <c r="J58" t="n">
-        <v>2.2</v>
+        <v>7.3</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Northern Illinois -11.0</t>
+          <t>Texas Tech -23.5</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>Northern Illinois -11.5</t>
+          <t>Texas Tech -23.5</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Northern Illinois -11.5</t>
+          <t>Texas Tech -23.6</t>
         </is>
       </c>
       <c r="O58" t="n">
-        <v>-11.5</v>
+        <v>23.6</v>
       </c>
       <c r="P58" t="n">
-        <v>-11.5</v>
+        <v>23.5</v>
       </c>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr"/>

</xml_diff>

<commit_message>
trying to fix team page and fixing spreads
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week12.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week12.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,59 +625,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9:30 PM</t>
+          <t>9:00 PM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>San Diego State</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>23.2</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
-        <v>24.8</v>
+        <v>21.8</v>
       </c>
       <c r="I3" t="n">
-        <v>42.2</v>
+        <v>55.32</v>
       </c>
       <c r="J3" t="n">
-        <v>8.199999999999999</v>
+        <v>8.1</v>
       </c>
       <c r="K3" t="n">
-        <v>4.7</v>
+        <v>5.2</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>San Diego State -2.5</t>
+          <t>Washington State -6.5</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>San Diego State -3.0</t>
+          <t>Washington State -8.5</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Boise State -1.7</t>
+          <t>Washington State -3.3</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>-1.7</v>
+        <v>3.3</v>
       </c>
       <c r="P3" t="n">
-        <v>3</v>
+        <v>8.5</v>
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
@@ -697,59 +697,59 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>9:30 PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>35.2</v>
+        <v>23.2</v>
       </c>
       <c r="H4" t="n">
-        <v>17.2</v>
+        <v>24.8</v>
       </c>
       <c r="I4" t="n">
-        <v>85.78</v>
+        <v>42.2</v>
       </c>
       <c r="J4" t="n">
-        <v>3.3</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>4.600000000000001</v>
+        <v>4.7</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Western Kentucky -14.0</t>
+          <t>San Diego State -2.5</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Western Kentucky -13.5</t>
+          <t>San Diego State -3.0</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Western Kentucky -18.1</t>
+          <t>Boise State -1.7</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>18.1</v>
+        <v>-1.7</v>
       </c>
       <c r="P4" t="n">
-        <v>13.5</v>
+        <v>3</v>
       </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
@@ -774,54 +774,54 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>37.9</v>
+        <v>35.2</v>
       </c>
       <c r="H5" t="n">
-        <v>18.9</v>
+        <v>17.2</v>
       </c>
       <c r="I5" t="n">
-        <v>86.70999999999999</v>
+        <v>85.78</v>
       </c>
       <c r="J5" t="n">
-        <v>7.9</v>
+        <v>3.3</v>
       </c>
       <c r="K5" t="n">
-        <v>4.5</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Miami -14.5</t>
+          <t>Western Kentucky -14.0</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Miami -14.5</t>
+          <t>Western Kentucky -13.5</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Miami -19.0</t>
+          <t>Western Kentucky -18.1</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>19</v>
+        <v>18.1</v>
       </c>
       <c r="P5" t="n">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
@@ -841,59 +841,59 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>25</v>
+        <v>37.9</v>
       </c>
       <c r="H6" t="n">
-        <v>21.8</v>
+        <v>18.9</v>
       </c>
       <c r="I6" t="n">
-        <v>55.32</v>
+        <v>86.70999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>8.1</v>
+        <v>7.9</v>
       </c>
       <c r="K6" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Washington State -6.5</t>
+          <t>Miami -14.5</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Washington State -7.5</t>
+          <t>Miami -14.5</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Washington State -3.3</t>
+          <t>Miami -19.0</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>3.3</v>
+        <v>19</v>
       </c>
       <c r="P6" t="n">
-        <v>7.5</v>
+        <v>14.5</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
@@ -985,59 +985,59 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Georgia State</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>26</v>
+        <v>35.7</v>
       </c>
       <c r="H8" t="n">
-        <v>37.2</v>
+        <v>17.6</v>
       </c>
       <c r="I8" t="n">
-        <v>20.81</v>
+        <v>85.92</v>
       </c>
       <c r="J8" t="n">
-        <v>3.4</v>
+        <v>6.7</v>
       </c>
       <c r="K8" t="n">
-        <v>4.199999999999999</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Marshall -6.5</t>
+          <t>Florida State -11.5</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Marshall -7.0</t>
+          <t>Florida State -14.0</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Marshall -11.2</t>
+          <t>Florida State -18.1</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>-11.2</v>
+        <v>18.1</v>
       </c>
       <c r="P8" t="n">
-        <v>-7</v>
+        <v>14</v>
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
@@ -1057,59 +1057,59 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oklahoma State</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>15.8</v>
+        <v>22.1</v>
       </c>
       <c r="H9" t="n">
-        <v>38.6</v>
+        <v>35</v>
       </c>
       <c r="I9" t="n">
-        <v>6.88</v>
+        <v>17.67</v>
       </c>
       <c r="J9" t="n">
-        <v>3.1</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>4.199999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Kansas State -20.0</t>
+          <t>Utah -9.0</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Kansas State -18.5</t>
+          <t>Utah -9.0</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Kansas State -22.7</t>
+          <t>Utah -12.9</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>-22.7</v>
+        <v>-12.9</v>
       </c>
       <c r="P9" t="n">
-        <v>-18.5</v>
+        <v>-9</v>
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
@@ -1129,59 +1129,59 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>1:00 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Georgia State</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>35.7</v>
+        <v>26</v>
       </c>
       <c r="H10" t="n">
-        <v>17.6</v>
+        <v>37.2</v>
       </c>
       <c r="I10" t="n">
-        <v>85.92</v>
+        <v>20.81</v>
       </c>
       <c r="J10" t="n">
-        <v>6.7</v>
+        <v>3.4</v>
       </c>
       <c r="K10" t="n">
-        <v>4.100000000000001</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Florida State -11.5</t>
+          <t>Marshall -6.5</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Florida State -14.0</t>
+          <t>Marshall -7.5</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Florida State -18.1</t>
+          <t>Marshall -11.2</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>18.1</v>
+        <v>-11.2</v>
       </c>
       <c r="P10" t="n">
-        <v>14</v>
+        <v>-7.5</v>
       </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
@@ -1232,7 +1232,7 @@
         <v>3.9</v>
       </c>
       <c r="K11" t="n">
-        <v>4.1</v>
+        <v>3.6</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Akron -5.0</t>
+          <t>Akron -5.5</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1253,7 +1253,7 @@
         <v>9.1</v>
       </c>
       <c r="P11" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
@@ -1273,59 +1273,59 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Northwestern</t>
+          <t>Tulsa</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>15.6</v>
+        <v>24.4</v>
       </c>
       <c r="H12" t="n">
-        <v>29.6</v>
+        <v>27</v>
       </c>
       <c r="I12" t="n">
-        <v>18.33</v>
+        <v>40.3</v>
       </c>
       <c r="J12" t="n">
-        <v>7.8</v>
+        <v>5.3</v>
       </c>
       <c r="K12" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Michigan -10.0</t>
+          <t>Oregon State -1.0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Michigan -10.0</t>
+          <t>Tulsa -1.0</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Michigan -14.0</t>
+          <t>Oregon State -2.5</t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>-14</v>
+        <v>-2.5</v>
       </c>
       <c r="P12" t="n">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
@@ -1345,59 +1345,59 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>9:15 PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>22.1</v>
+        <v>30.2</v>
       </c>
       <c r="H13" t="n">
-        <v>35</v>
+        <v>22.5</v>
       </c>
       <c r="I13" t="n">
-        <v>17.67</v>
+        <v>66.98999999999999</v>
       </c>
       <c r="J13" t="n">
-        <v>8.199999999999999</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K13" t="n">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Utah -9.0</t>
+          <t>BYU -6.0</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Utah -9.0</t>
+          <t>BYU -4.5</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Utah -12.9</t>
+          <t>BYU -7.8</t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>-12.9</v>
+        <v>7.8</v>
       </c>
       <c r="P13" t="n">
-        <v>-9</v>
+        <v>4.5</v>
       </c>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
@@ -1417,59 +1417,59 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>3:15 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Tulsa</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>24.4</v>
+        <v>46.7</v>
       </c>
       <c r="H14" t="n">
-        <v>27</v>
+        <v>10.5</v>
       </c>
       <c r="I14" t="n">
-        <v>40.3</v>
+        <v>97.8</v>
       </c>
       <c r="J14" t="n">
-        <v>5.3</v>
+        <v>2.9</v>
       </c>
       <c r="K14" t="n">
-        <v>3.5</v>
+        <v>3.299999999999997</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Oregon State -1.0</t>
+          <t>Tennessee -38.5</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Tulsa -1.0</t>
+          <t>Tennessee -39.5</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Oregon State -2.5</t>
+          <t>Tennessee -36.2</t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>-2.5</v>
+        <v>36.2</v>
       </c>
       <c r="P14" t="n">
-        <v>1</v>
+        <v>39.5</v>
       </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
@@ -1485,63 +1485,63 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>UCLA</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>36.8</v>
+        <v>43.2</v>
       </c>
       <c r="H15" t="n">
-        <v>9.5</v>
+        <v>8.4</v>
       </c>
       <c r="I15" t="n">
-        <v>94.25</v>
+        <v>97.38</v>
       </c>
       <c r="J15" t="n">
-        <v>6.7</v>
+        <v>5.3</v>
       </c>
       <c r="K15" t="n">
-        <v>3.300000000000001</v>
+        <v>3.200000000000003</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Oregon -23.0</t>
+          <t>Ohio State -31.5</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Oregon -24.0</t>
+          <t>Ohio State -31.5</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Oregon -27.3</t>
+          <t>Ohio State -34.7</t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>27.3</v>
+        <v>34.7</v>
       </c>
       <c r="P15" t="n">
-        <v>24</v>
+        <v>31.5</v>
       </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
@@ -1561,59 +1561,59 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3:15 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>New Mexico State</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>46.7</v>
+        <v>15.8</v>
       </c>
       <c r="H16" t="n">
-        <v>10.5</v>
+        <v>38.6</v>
       </c>
       <c r="I16" t="n">
-        <v>97.8</v>
+        <v>6.88</v>
       </c>
       <c r="J16" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="K16" t="n">
-        <v>3.299999999999997</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Tennessee -38.5</t>
+          <t>Kansas State -20.0</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Tennessee -39.5</t>
+          <t>Kansas State -19.5</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Tennessee -36.2</t>
+          <t>Kansas State -22.7</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>36.2</v>
+        <v>-22.7</v>
       </c>
       <c r="P16" t="n">
-        <v>39.5</v>
+        <v>-19.5</v>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
@@ -1633,59 +1633,59 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>UCLA</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>43.2</v>
+        <v>39.8</v>
       </c>
       <c r="H17" t="n">
-        <v>8.4</v>
+        <v>6.6</v>
       </c>
       <c r="I17" t="n">
-        <v>97.38</v>
+        <v>96.88</v>
       </c>
       <c r="J17" t="n">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
       <c r="K17" t="n">
-        <v>3.200000000000003</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Ohio State -31.5</t>
+          <t>Indiana -30.5</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Ohio State -31.5</t>
+          <t>Indiana -30.0</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Ohio State -34.7</t>
+          <t>Indiana -33.1</t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>34.7</v>
+        <v>33.1</v>
       </c>
       <c r="P17" t="n">
-        <v>31.5</v>
+        <v>30</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -1705,59 +1705,59 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>3:30 PM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>The CW Network</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>39.8</v>
+        <v>25.6</v>
       </c>
       <c r="H18" t="n">
-        <v>6.6</v>
+        <v>16</v>
       </c>
       <c r="I18" t="n">
-        <v>96.88</v>
+        <v>71.06999999999999</v>
       </c>
       <c r="J18" t="n">
-        <v>5.4</v>
+        <v>7.2</v>
       </c>
       <c r="K18" t="n">
-        <v>3.100000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Indiana -30.5</t>
+          <t>Wake Forest -6.0</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Indiana -30.0</t>
+          <t>Wake Forest -6.5</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Indiana -33.1</t>
+          <t>Wake Forest -9.6</t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>33.1</v>
+        <v>9.6</v>
       </c>
       <c r="P18" t="n">
-        <v>30</v>
+        <v>6.5</v>
       </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
@@ -1777,59 +1777,59 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3:30 PM</t>
+          <t>12:00 PM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>The CW Network</t>
+          <t>TNT</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>25.6</v>
+        <v>32.4</v>
       </c>
       <c r="H19" t="n">
-        <v>16</v>
+        <v>17.8</v>
       </c>
       <c r="I19" t="n">
-        <v>71.06999999999999</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="J19" t="n">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="K19" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Wake Forest -6.0</t>
+          <t>Arizona State -11.0</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Wake Forest -6.5</t>
+          <t>Arizona State -11.5</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Wake Forest -9.6</t>
+          <t>Arizona State -14.5</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>9.6</v>
+        <v>14.5</v>
       </c>
       <c r="P19" t="n">
-        <v>6.5</v>
+        <v>11.5</v>
       </c>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
@@ -1849,59 +1849,59 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12:00 PM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Kennesaw State</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>32.4</v>
+        <v>25.2</v>
       </c>
       <c r="H20" t="n">
-        <v>17.8</v>
+        <v>25.6</v>
       </c>
       <c r="I20" t="n">
-        <v>80.09999999999999</v>
+        <v>43.3</v>
       </c>
       <c r="J20" t="n">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="K20" t="n">
         <v>3</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Arizona State -11.0</t>
+          <t>Kennesaw State -2.5</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Arizona State -11.5</t>
+          <t>Kennesaw State -3.5</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Arizona State -14.5</t>
+          <t>Kennesaw State -0.5</t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>14.5</v>
+        <v>-0.5</v>
       </c>
       <c r="P20" t="n">
-        <v>11.5</v>
+        <v>-3.5</v>
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
@@ -1921,59 +1921,59 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Utah State</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>37.1</v>
+        <v>30.4</v>
       </c>
       <c r="H21" t="n">
-        <v>29.7</v>
+        <v>27.2</v>
       </c>
       <c r="I21" t="n">
-        <v>64.70999999999999</v>
+        <v>54.48</v>
       </c>
       <c r="J21" t="n">
-        <v>7.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K21" t="n">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>UNLV -4.5</t>
+          <t>Duke -6.5</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>UNLV -4.5</t>
+          <t>Duke -6.0</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>UNLV -7.4</t>
+          <t>Duke -3.3</t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>7.4</v>
+        <v>3.3</v>
       </c>
       <c r="P21" t="n">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
@@ -1993,59 +1993,59 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Northwestern</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>App State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>38.5</v>
+        <v>15.6</v>
       </c>
       <c r="H22" t="n">
-        <v>15.7</v>
+        <v>29.6</v>
       </c>
       <c r="I22" t="n">
-        <v>90.81999999999999</v>
+        <v>18.33</v>
       </c>
       <c r="J22" t="n">
-        <v>4.6</v>
+        <v>7.8</v>
       </c>
       <c r="K22" t="n">
-        <v>2.800000000000001</v>
+        <v>2.5</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>James Madison -19.5</t>
+          <t>Michigan -10.0</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>James Madison -20.0</t>
+          <t>Michigan -11.5</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>James Madison -22.8</t>
+          <t>Michigan -14.0</t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>22.8</v>
+        <v>-14</v>
       </c>
       <c r="P22" t="n">
-        <v>20</v>
+        <v>-11.5</v>
       </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
@@ -2065,59 +2065,59 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Air Force</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>30.4</v>
+        <v>36.2</v>
       </c>
       <c r="H23" t="n">
-        <v>27.2</v>
+        <v>26.8</v>
       </c>
       <c r="I23" t="n">
-        <v>54.48</v>
+        <v>69.66</v>
       </c>
       <c r="J23" t="n">
-        <v>9.199999999999999</v>
+        <v>7</v>
       </c>
       <c r="K23" t="n">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Duke -6.5</t>
+          <t>UConn -8.0</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Duke -6.0</t>
+          <t>UConn -7.0</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Duke -3.3</t>
+          <t>UConn -9.4</t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>3.3</v>
+        <v>9.4</v>
       </c>
       <c r="P23" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
@@ -2133,63 +2133,63 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>11:45 AM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>SEC Network</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>19.6</v>
+        <v>32.7</v>
       </c>
       <c r="H24" t="n">
-        <v>25.6</v>
+        <v>25.4</v>
       </c>
       <c r="I24" t="n">
-        <v>30.82</v>
+        <v>64.97</v>
       </c>
       <c r="J24" t="n">
-        <v>6.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K24" t="n">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Toledo -3.0</t>
+          <t>LSU -6.5</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Toledo -3.5</t>
+          <t>LSU -5.0</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Toledo -6.1</t>
+          <t>LSU -7.3</t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>-6.1</v>
+        <v>7.3</v>
       </c>
       <c r="P24" t="n">
-        <v>-3.5</v>
+        <v>5</v>
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -2209,59 +2209,59 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Cincinnati</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Kennesaw State</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>25.2</v>
+        <v>29.8</v>
       </c>
       <c r="H25" t="n">
-        <v>25.6</v>
+        <v>26.2</v>
       </c>
       <c r="I25" t="n">
-        <v>43.3</v>
+        <v>56.15</v>
       </c>
       <c r="J25" t="n">
-        <v>6.7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K25" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Kennesaw State -2.5</t>
+          <t>Cincinnati -6.0</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Kennesaw State -3.0</t>
+          <t>Cincinnati -6.0</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Kennesaw State -0.5</t>
+          <t>Cincinnati -3.7</t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>-0.5</v>
+        <v>3.7</v>
       </c>
       <c r="P25" t="n">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -2277,63 +2277,63 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45976</v>
+        <v>45973</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>36.2</v>
+        <v>19.6</v>
       </c>
       <c r="H26" t="n">
-        <v>26.8</v>
+        <v>25.6</v>
       </c>
       <c r="I26" t="n">
-        <v>69.66</v>
+        <v>30.82</v>
       </c>
       <c r="J26" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="K26" t="n">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>UConn -8.0</t>
+          <t>Toledo -3.0</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>UConn -7.0</t>
+          <t>Toledo -4.0</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>UConn -9.4</t>
+          <t>Toledo -6.1</t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>9.4</v>
+        <v>-6.1</v>
       </c>
       <c r="P26" t="n">
-        <v>7</v>
+        <v>-4</v>
       </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2363,49 +2363,49 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>23</v>
+        <v>22.3</v>
       </c>
       <c r="H27" t="n">
-        <v>43.4</v>
+        <v>33.7</v>
       </c>
       <c r="I27" t="n">
-        <v>8.640000000000001</v>
+        <v>23.11</v>
       </c>
       <c r="J27" t="n">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="K27" t="n">
-        <v>2.399999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>North Texas -18.0</t>
+          <t>Delaware -8.5</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>North Texas -18.0</t>
+          <t>Delaware -9.5</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>North Texas -20.4</t>
+          <t>Delaware -11.4</t>
         </is>
       </c>
       <c r="O27" t="n">
-        <v>-20.4</v>
+        <v>-11.4</v>
       </c>
       <c r="P27" t="n">
-        <v>-18</v>
+        <v>-9.5</v>
       </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
@@ -2421,63 +2421,63 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Cincinnati</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>29.8</v>
+        <v>36.8</v>
       </c>
       <c r="H28" t="n">
-        <v>26.2</v>
+        <v>9.5</v>
       </c>
       <c r="I28" t="n">
-        <v>56.15</v>
+        <v>94.25</v>
       </c>
       <c r="J28" t="n">
-        <v>9.300000000000001</v>
+        <v>6.7</v>
       </c>
       <c r="K28" t="n">
-        <v>2.3</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Cincinnati -6.0</t>
+          <t>Oregon -23.0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Cincinnati -6.0</t>
+          <t>Oregon -25.5</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Cincinnati -3.7</t>
+          <t>Oregon -27.3</t>
         </is>
       </c>
       <c r="O28" t="n">
-        <v>3.7</v>
+        <v>27.3</v>
       </c>
       <c r="P28" t="n">
-        <v>6</v>
+        <v>25.5</v>
       </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
@@ -2497,59 +2497,59 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>9:15 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>App State</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>30.2</v>
+        <v>38.5</v>
       </c>
       <c r="H29" t="n">
-        <v>22.5</v>
+        <v>15.7</v>
       </c>
       <c r="I29" t="n">
-        <v>66.98999999999999</v>
+        <v>90.81999999999999</v>
       </c>
       <c r="J29" t="n">
-        <v>9.199999999999999</v>
+        <v>4.6</v>
       </c>
       <c r="K29" t="n">
-        <v>2.3</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>BYU -6.0</t>
+          <t>James Madison -19.5</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>BYU -5.5</t>
+          <t>James Madison -21.0</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>BYU -7.8</t>
+          <t>James Madison -22.8</t>
         </is>
       </c>
       <c r="O29" t="n">
-        <v>7.8</v>
+        <v>22.8</v>
       </c>
       <c r="P29" t="n">
-        <v>5.5</v>
+        <v>21</v>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
@@ -2569,59 +2569,59 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ESPNU</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>30</v>
+        <v>35.6</v>
       </c>
       <c r="H30" t="n">
-        <v>29.2</v>
+        <v>16.8</v>
       </c>
       <c r="I30" t="n">
-        <v>48.88</v>
+        <v>86.45</v>
       </c>
       <c r="J30" t="n">
-        <v>9</v>
+        <v>6.8</v>
       </c>
       <c r="K30" t="n">
-        <v>2.1</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>East Carolina -3.0</t>
+          <t>Washington -16.5</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>East Carolina -3.0</t>
+          <t>Washington -17.0</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>East Carolina -0.9</t>
+          <t>Washington -18.8</t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>0.9</v>
+        <v>18.8</v>
       </c>
       <c r="P30" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
@@ -2641,59 +2641,59 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>9:30 PM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>22.3</v>
+        <v>25.8</v>
       </c>
       <c r="H31" t="n">
-        <v>33.7</v>
+        <v>20.6</v>
       </c>
       <c r="I31" t="n">
-        <v>23.11</v>
+        <v>59.7</v>
       </c>
       <c r="J31" t="n">
-        <v>3.2</v>
+        <v>7.3</v>
       </c>
       <c r="K31" t="n">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Delaware -8.5</t>
+          <t>Fresno State -4.0</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Delaware -9.5</t>
+          <t>Fresno State -3.5</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Delaware -11.4</t>
+          <t>Fresno State -5.2</t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>-11.4</v>
+        <v>5.2</v>
       </c>
       <c r="P31" t="n">
-        <v>-9.5</v>
+        <v>3.5</v>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2713,59 +2713,59 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPNU</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>UL Monroe</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>24.2</v>
+        <v>30</v>
       </c>
       <c r="H32" t="n">
-        <v>30</v>
+        <v>29.2</v>
       </c>
       <c r="I32" t="n">
-        <v>32.27</v>
+        <v>48.88</v>
       </c>
       <c r="J32" t="n">
-        <v>4.1</v>
+        <v>9</v>
       </c>
       <c r="K32" t="n">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>South Alabama -4.0</t>
+          <t>East Carolina -3.0</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>South Alabama -4.0</t>
+          <t>East Carolina -2.5</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>South Alabama -5.9</t>
+          <t>East Carolina -0.9</t>
         </is>
       </c>
       <c r="O32" t="n">
-        <v>-5.9</v>
+        <v>0.9</v>
       </c>
       <c r="P32" t="n">
-        <v>-4</v>
+        <v>2.5</v>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
@@ -2785,59 +2785,59 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>UTEP</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>35.6</v>
+        <v>27.8</v>
       </c>
       <c r="H33" t="n">
-        <v>16.8</v>
+        <v>22.2</v>
       </c>
       <c r="I33" t="n">
-        <v>86.45</v>
+        <v>60.51</v>
       </c>
       <c r="J33" t="n">
-        <v>6.8</v>
+        <v>5.8</v>
       </c>
       <c r="K33" t="n">
-        <v>1.800000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Washington -16.5</t>
+          <t>Missouri State -4.0</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Washington -17.0</t>
+          <t>Missouri State -4.0</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Washington -18.8</t>
+          <t>Missouri State -5.6</t>
         </is>
       </c>
       <c r="O33" t="n">
-        <v>18.8</v>
+        <v>5.6</v>
       </c>
       <c r="P33" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -2853,7 +2853,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45973</v>
+        <v>45976</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -2867,49 +2867,49 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Utah State</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>22.2</v>
+        <v>37.1</v>
       </c>
       <c r="H34" t="n">
-        <v>21.5</v>
+        <v>29.7</v>
       </c>
       <c r="I34" t="n">
-        <v>49.16</v>
+        <v>64.70999999999999</v>
       </c>
       <c r="J34" t="n">
-        <v>6.7</v>
+        <v>7.6</v>
       </c>
       <c r="K34" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Central Michigan -2.0</t>
+          <t>UNLV -4.5</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Central Michigan -2.5</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Central Michigan -0.8</t>
+          <t>UNLV -7.4</t>
         </is>
       </c>
       <c r="O34" t="n">
-        <v>0.8</v>
+        <v>7.4</v>
       </c>
       <c r="P34" t="n">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2939,49 +2939,49 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>20.8</v>
+        <v>24.2</v>
       </c>
       <c r="H35" t="n">
-        <v>39.9</v>
+        <v>30</v>
       </c>
       <c r="I35" t="n">
-        <v>9.859999999999999</v>
+        <v>32.27</v>
       </c>
       <c r="J35" t="n">
-        <v>2.5</v>
+        <v>4.1</v>
       </c>
       <c r="K35" t="n">
-        <v>1.600000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>UTSA -18.0</t>
+          <t>South Alabama -4.0</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>UTSA -17.5</t>
+          <t>South Alabama -4.5</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>UTSA -19.1</t>
+          <t>South Alabama -5.9</t>
         </is>
       </c>
       <c r="O35" t="n">
-        <v>-19.1</v>
+        <v>-5.9</v>
       </c>
       <c r="P35" t="n">
-        <v>-17.5</v>
+        <v>-4.5</v>
       </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>1:00 PM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3011,49 +3011,49 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>UTEP</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>27.8</v>
+        <v>23</v>
       </c>
       <c r="H36" t="n">
-        <v>22.2</v>
+        <v>43.4</v>
       </c>
       <c r="I36" t="n">
-        <v>60.51</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="J36" t="n">
-        <v>5.8</v>
+        <v>3.6</v>
       </c>
       <c r="K36" t="n">
-        <v>1.6</v>
+        <v>1.399999999999999</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Missouri State -4.0</t>
+          <t>North Texas -18.0</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Missouri State -4.0</t>
+          <t>North Texas -19.0</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Missouri State -5.6</t>
+          <t>North Texas -20.4</t>
         </is>
       </c>
       <c r="O36" t="n">
-        <v>5.6</v>
+        <v>-20.4</v>
       </c>
       <c r="P36" t="n">
-        <v>4</v>
+        <v>-19</v>
       </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
@@ -3073,59 +3073,59 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>11:45 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>SEC Network</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>32.7</v>
+        <v>33.1</v>
       </c>
       <c r="H37" t="n">
-        <v>25.4</v>
+        <v>18.3</v>
       </c>
       <c r="I37" t="n">
-        <v>64.97</v>
+        <v>80.28</v>
       </c>
       <c r="J37" t="n">
-        <v>9.199999999999999</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="K37" t="n">
-        <v>1.3</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>LSU -6.5</t>
+          <t>Ole Miss -14.0</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>LSU -6.0</t>
+          <t>Ole Miss -16.0</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>LSU -7.3</t>
+          <t>Ole Miss -14.8</t>
         </is>
       </c>
       <c r="O37" t="n">
-        <v>7.3</v>
+        <v>14.8</v>
       </c>
       <c r="P37" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
@@ -3141,11 +3141,11 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45976</v>
+        <v>45974</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3155,49 +3155,49 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>33.1</v>
+        <v>32.6</v>
       </c>
       <c r="H38" t="n">
-        <v>18.3</v>
+        <v>22.4</v>
       </c>
       <c r="I38" t="n">
-        <v>80.28</v>
+        <v>72.66</v>
       </c>
       <c r="J38" t="n">
-        <v>8.699999999999999</v>
+        <v>6.9</v>
       </c>
       <c r="K38" t="n">
         <v>1.199999999999999</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Ole Miss -14.0</t>
+          <t>Old Dominion -11.5</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Ole Miss -16.0</t>
+          <t>Old Dominion -11.5</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Ole Miss -14.8</t>
+          <t>Old Dominion -10.3</t>
         </is>
       </c>
       <c r="O38" t="n">
-        <v>14.8</v>
+        <v>10.3</v>
       </c>
       <c r="P38" t="n">
-        <v>16</v>
+        <v>11.5</v>
       </c>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
@@ -3289,59 +3289,59 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>2:00 PM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>CBSSN</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>21.4</v>
+        <v>35</v>
       </c>
       <c r="H40" t="n">
-        <v>30.4</v>
+        <v>21.6</v>
       </c>
       <c r="I40" t="n">
-        <v>24.96</v>
+        <v>78.06</v>
       </c>
       <c r="J40" t="n">
-        <v>3.9</v>
+        <v>5.1</v>
       </c>
       <c r="K40" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>San José State -8.5</t>
+          <t>New Mexico -12.5</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>San José State -8.0</t>
+          <t>New Mexico -14.5</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>San José State -9.0</t>
+          <t>New Mexico -13.4</t>
         </is>
       </c>
       <c r="O40" t="n">
-        <v>-9</v>
+        <v>13.4</v>
       </c>
       <c r="P40" t="n">
-        <v>-8</v>
+        <v>14.5</v>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -3429,63 +3429,63 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45972</v>
+        <v>45976</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>24.3</v>
+        <v>32.1</v>
       </c>
       <c r="H42" t="n">
-        <v>24.9</v>
+        <v>28.6</v>
       </c>
       <c r="I42" t="n">
-        <v>45.8</v>
+        <v>55.32</v>
       </c>
       <c r="J42" t="n">
-        <v>7.1</v>
+        <v>6.7</v>
       </c>
       <c r="K42" t="n">
-        <v>0.9</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Ohio -1.5</t>
+          <t>Georgia Southern -3.0</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Ohio -1.5</t>
+          <t>Georgia Southern -2.5</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Ohio -0.6</t>
+          <t>Georgia Southern -3.4</t>
         </is>
       </c>
       <c r="O42" t="n">
-        <v>-0.6</v>
+        <v>3.4</v>
       </c>
       <c r="P42" t="n">
-        <v>-1.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
@@ -3501,63 +3501,63 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>6:30 PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>ESPN</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>32.1</v>
+        <v>28</v>
       </c>
       <c r="H43" t="n">
-        <v>28.6</v>
+        <v>24</v>
       </c>
       <c r="I43" t="n">
-        <v>55.32</v>
+        <v>56.7</v>
       </c>
       <c r="J43" t="n">
-        <v>6.7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K43" t="n">
         <v>0.8999999999999999</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.0</t>
+          <t>Louisville -3.5</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Georgia Southern -2.5</t>
+          <t>Louisville -3.0</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.4</t>
+          <t>Louisville -3.9</t>
         </is>
       </c>
       <c r="O43" t="n">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="P43" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
@@ -3577,59 +3577,59 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ESPN2</t>
+          <t>FS1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>26.4</v>
+        <v>34.4</v>
       </c>
       <c r="H44" t="n">
-        <v>36.2</v>
+        <v>19.8</v>
       </c>
       <c r="I44" t="n">
-        <v>23.32</v>
+        <v>80.81</v>
       </c>
       <c r="J44" t="n">
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
       <c r="K44" t="n">
         <v>0.8000000000000007</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>South Florida -10.0</t>
+          <t>Illinois -14.0</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>South Florida -10.5</t>
+          <t>Illinois -15.5</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>South Florida -9.7</t>
+          <t>Illinois -14.7</t>
         </is>
       </c>
       <c r="O44" t="n">
-        <v>-9.699999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="P44" t="n">
-        <v>-10.5</v>
+        <v>15.5</v>
       </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -3649,59 +3649,59 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>9:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Wyoming</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>25.8</v>
+        <v>26.4</v>
       </c>
       <c r="H45" t="n">
-        <v>20.6</v>
+        <v>36.2</v>
       </c>
       <c r="I45" t="n">
-        <v>59.7</v>
+        <v>23.32</v>
       </c>
       <c r="J45" t="n">
         <v>7.3</v>
       </c>
       <c r="K45" t="n">
-        <v>0.7000000000000002</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Fresno State -4.0</t>
+          <t>South Florida -10.0</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Fresno State -4.5</t>
+          <t>South Florida -10.5</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Fresno State -5.2</t>
+          <t>South Florida -9.7</t>
         </is>
       </c>
       <c r="O45" t="n">
-        <v>5.2</v>
+        <v>-9.699999999999999</v>
       </c>
       <c r="P45" t="n">
-        <v>4.5</v>
+        <v>-10.5</v>
       </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
@@ -3726,54 +3726,54 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>FS1</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>34.4</v>
+        <v>27.2</v>
       </c>
       <c r="H46" t="n">
-        <v>19.8</v>
+        <v>20.5</v>
       </c>
       <c r="I46" t="n">
-        <v>80.81</v>
+        <v>62.9</v>
       </c>
       <c r="J46" t="n">
-        <v>7.8</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K46" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Illinois -14.0</t>
+          <t>Alabama -7.0</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Illinois -14.0</t>
+          <t>Alabama -6.0</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Illinois -14.7</t>
+          <t>Alabama -6.7</t>
         </is>
       </c>
       <c r="O46" t="n">
-        <v>14.7</v>
+        <v>6.7</v>
       </c>
       <c r="P46" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
@@ -3798,54 +3798,54 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>22.4</v>
+        <v>20.8</v>
       </c>
       <c r="H47" t="n">
-        <v>33.3</v>
+        <v>39.9</v>
       </c>
       <c r="I47" t="n">
-        <v>21.56</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="J47" t="n">
-        <v>8.9</v>
+        <v>2.5</v>
       </c>
       <c r="K47" t="n">
-        <v>0.5999999999999996</v>
+        <v>0.6000000000000014</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Notre Dame -10.5</t>
+          <t>UTSA -18.0</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Notre Dame -11.5</t>
+          <t>UTSA -18.5</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Notre Dame -10.9</t>
+          <t>UTSA -19.1</t>
         </is>
       </c>
       <c r="O47" t="n">
-        <v>-10.9</v>
+        <v>-19.1</v>
       </c>
       <c r="P47" t="n">
-        <v>-11.5</v>
+        <v>-18.5</v>
       </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
@@ -3865,59 +3865,59 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>2:30 PM</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>27.8</v>
+        <v>21.4</v>
       </c>
       <c r="H48" t="n">
-        <v>21.4</v>
+        <v>30.4</v>
       </c>
       <c r="I48" t="n">
-        <v>62.64</v>
+        <v>24.96</v>
       </c>
       <c r="J48" t="n">
-        <v>9.699999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="K48" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Georgia -6.5</t>
+          <t>San José State -8.5</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Georgia -6.0</t>
+          <t>San José State -9.5</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Georgia -6.4</t>
+          <t>San José State -9.0</t>
         </is>
       </c>
       <c r="O48" t="n">
-        <v>6.4</v>
+        <v>-9</v>
       </c>
       <c r="P48" t="n">
-        <v>6</v>
+        <v>-9.5</v>
       </c>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
@@ -3933,7 +3933,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45975</v>
+        <v>45976</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -3942,54 +3942,54 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>28</v>
+        <v>27.8</v>
       </c>
       <c r="H49" t="n">
-        <v>24</v>
+        <v>21.4</v>
       </c>
       <c r="I49" t="n">
-        <v>56.7</v>
+        <v>62.64</v>
       </c>
       <c r="J49" t="n">
-        <v>9.300000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K49" t="n">
-        <v>0.3999999999999999</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Louisville -3.5</t>
+          <t>Georgia -6.5</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Louisville -3.5</t>
+          <t>Georgia -6.0</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Louisville -3.9</t>
+          <t>Georgia -6.4</t>
         </is>
       </c>
       <c r="O49" t="n">
-        <v>3.9</v>
+        <v>6.4</v>
       </c>
       <c r="P49" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
@@ -4005,63 +4005,63 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45976</v>
+        <v>45972</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>11:00 AM</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ESPN</t>
+          <t>ESPN2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>35.1</v>
+        <v>24.3</v>
       </c>
       <c r="H50" t="n">
-        <v>15.8</v>
+        <v>24.9</v>
       </c>
       <c r="I50" t="n">
-        <v>87.34999999999999</v>
+        <v>45.8</v>
       </c>
       <c r="J50" t="n">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="K50" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.4</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -18.5</t>
+          <t>Ohio -1.5</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -19.0</t>
+          <t>Ohio -1.0</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -19.3</t>
+          <t>Ohio -0.6</t>
         </is>
       </c>
       <c r="O50" t="n">
-        <v>19.3</v>
+        <v>-0.6</v>
       </c>
       <c r="P50" t="n">
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
@@ -4086,54 +4086,54 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ACC Network</t>
+          <t>FOX</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>21</v>
+        <v>36.3</v>
       </c>
       <c r="H51" t="n">
-        <v>37.8</v>
+        <v>12.7</v>
       </c>
       <c r="I51" t="n">
-        <v>12.29</v>
+        <v>91.62</v>
       </c>
       <c r="J51" t="n">
-        <v>5</v>
+        <v>7.3</v>
       </c>
       <c r="K51" t="n">
-        <v>0.3000000000000007</v>
+        <v>0.3999999999999986</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Georgia Tech -16.5</t>
+          <t>Texas Tech -23.5</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Georgia Tech -17.0</t>
+          <t>Texas Tech -24.0</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Georgia Tech -16.7</t>
+          <t>Texas Tech -23.6</t>
         </is>
       </c>
       <c r="O51" t="n">
-        <v>-16.7</v>
+        <v>23.6</v>
       </c>
       <c r="P51" t="n">
-        <v>-17</v>
+        <v>24</v>
       </c>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
@@ -4153,59 +4153,59 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2:30 PM</t>
+          <t>3:00 PM</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Florida Atlantic</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>29.6</v>
+        <v>39</v>
       </c>
       <c r="H52" t="n">
-        <v>23.4</v>
+        <v>21.8</v>
       </c>
       <c r="I52" t="n">
-        <v>62.9</v>
+        <v>84.34999999999999</v>
       </c>
       <c r="J52" t="n">
-        <v>9.6</v>
+        <v>5.2</v>
       </c>
       <c r="K52" t="n">
-        <v>0.2999999999999998</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>USC -6.5</t>
+          <t>Tulane -16.5</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>USC -6.5</t>
+          <t>Tulane -17.5</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>USC -6.2</t>
+          <t>Tulane -17.2</t>
         </is>
       </c>
       <c r="O52" t="n">
-        <v>6.2</v>
+        <v>17.2</v>
       </c>
       <c r="P52" t="n">
-        <v>6.5</v>
+        <v>17.5</v>
       </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
@@ -4230,54 +4230,54 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Southern Miss</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>34.6</v>
+        <v>29.6</v>
       </c>
       <c r="H53" t="n">
-        <v>28.9</v>
+        <v>23.4</v>
       </c>
       <c r="I53" t="n">
-        <v>62.37</v>
+        <v>62.9</v>
       </c>
       <c r="J53" t="n">
-        <v>7.3</v>
+        <v>9.6</v>
       </c>
       <c r="K53" t="n">
         <v>0.2999999999999998</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Southern Miss -6.5</t>
+          <t>USC -6.5</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Southern Miss -6.0</t>
+          <t>USC -6.5</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Southern Miss -5.7</t>
+          <t>USC -6.2</t>
         </is>
       </c>
       <c r="O53" t="n">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
       <c r="P53" t="n">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
@@ -4374,54 +4374,54 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ESPN+</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Southern Miss</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>27.2</v>
+        <v>34.6</v>
       </c>
       <c r="H55" t="n">
-        <v>20.5</v>
+        <v>28.9</v>
       </c>
       <c r="I55" t="n">
-        <v>62.9</v>
+        <v>62.37</v>
       </c>
       <c r="J55" t="n">
-        <v>9.699999999999999</v>
+        <v>7.3</v>
       </c>
       <c r="K55" t="n">
         <v>0.2000000000000002</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Alabama -7.0</t>
+          <t>Southern Miss -6.5</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Alabama -6.5</t>
+          <t>Southern Miss -5.5</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Alabama -6.7</t>
+          <t>Southern Miss -5.7</t>
         </is>
       </c>
       <c r="O55" t="n">
-        <v>6.7</v>
+        <v>5.7</v>
       </c>
       <c r="P55" t="n">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
@@ -4437,63 +4437,63 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45976</v>
+        <v>45973</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>3:00 PM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ESPN+</t>
+          <t>CBSSN</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Central Michigan</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Florida Atlantic</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>39</v>
+        <v>22.2</v>
       </c>
       <c r="H56" t="n">
-        <v>21.8</v>
+        <v>21.5</v>
       </c>
       <c r="I56" t="n">
-        <v>84.34999999999999</v>
+        <v>49.16</v>
       </c>
       <c r="J56" t="n">
-        <v>5.2</v>
+        <v>6.7</v>
       </c>
       <c r="K56" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.2</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Tulane -16.5</t>
+          <t>Central Michigan -2.0</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Tulane -17.0</t>
+          <t>Central Michigan -1.0</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Tulane -17.2</t>
+          <t>Central Michigan -0.8</t>
         </is>
       </c>
       <c r="O56" t="n">
-        <v>17.2</v>
+        <v>0.8</v>
       </c>
       <c r="P56" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr"/>
@@ -4509,11 +4509,11 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>45974</v>
+        <v>45976</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6:30 PM</t>
+          <t>11:00 AM</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4523,49 +4523,49 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Old Dominion</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>32.6</v>
+        <v>35.1</v>
       </c>
       <c r="H57" t="n">
-        <v>22.4</v>
+        <v>15.8</v>
       </c>
       <c r="I57" t="n">
-        <v>72.66</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="J57" t="n">
-        <v>6.9</v>
+        <v>8.1</v>
       </c>
       <c r="K57" t="n">
         <v>0.1999999999999993</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Old Dominion -10.0</t>
+          <t>Texas A&amp;M -18.5</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Old Dominion -10.5</t>
+          <t>Texas A&amp;M -19.5</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Old Dominion -10.3</t>
+          <t>Texas A&amp;M -19.3</t>
         </is>
       </c>
       <c r="O57" t="n">
-        <v>10.3</v>
+        <v>19.3</v>
       </c>
       <c r="P57" t="n">
-        <v>10.5</v>
+        <v>19.5</v>
       </c>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr"/>
@@ -4590,54 +4590,54 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>ACC Network</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>36.3</v>
+        <v>21</v>
       </c>
       <c r="H58" t="n">
-        <v>12.7</v>
+        <v>37.8</v>
       </c>
       <c r="I58" t="n">
-        <v>91.62</v>
+        <v>12.29</v>
       </c>
       <c r="J58" t="n">
-        <v>7.3</v>
+        <v>5</v>
       </c>
       <c r="K58" t="n">
-        <v>0.1000000000000014</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Texas Tech -23.5</t>
+          <t>Georgia Tech -16.5</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>Texas Tech -23.5</t>
+          <t>Georgia Tech -16.5</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Texas Tech -23.6</t>
+          <t>Georgia Tech -16.7</t>
         </is>
       </c>
       <c r="O58" t="n">
-        <v>23.6</v>
+        <v>-16.7</v>
       </c>
       <c r="P58" t="n">
-        <v>23.5</v>
+        <v>-16.5</v>
       </c>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr"/>
@@ -4648,6 +4648,78 @@
         <v>0</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>11:00 AM</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Notre Dame</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="H59" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="I59" t="n">
+        <v>21.56</v>
+      </c>
+      <c r="J59" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.09999999999999964</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Notre Dame -10.5</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Notre Dame -11.0</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Notre Dame -10.9</t>
+        </is>
+      </c>
+      <c r="O59" t="n">
+        <v>-10.9</v>
+      </c>
+      <c r="P59" t="n">
+        <v>-11</v>
+      </c>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>